<commit_message>
feat: fill field values recursively
</commit_message>
<xml_diff>
--- a/tests/Test.xlsx
+++ b/tests/Test.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wenchyzhu/Github/tableau/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B7E21D-2AB5-934D-8048-06ADE565B0D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852A33B6-D0D8-F94D-A9D0-00558EF3C2F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="1060" yWindow="1620" windowWidth="28040" windowHeight="14740" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Activity" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>道具ID</t>
   </si>
@@ -42,15 +42,9 @@
     <t>描述</t>
   </si>
   <si>
-    <t>奖励池ID</t>
-  </si>
-  <si>
     <t>过期时间</t>
   </si>
   <si>
-    <t>属性列表</t>
-  </si>
-  <si>
     <t>1,2,3,4,5</t>
   </si>
   <si>
@@ -60,16 +54,79 @@
     <t>金币</t>
   </si>
   <si>
-    <t>道具ID1</t>
-  </si>
-  <si>
-    <t>道具NUM1</t>
-  </si>
-  <si>
-    <t>道具ID2</t>
-  </si>
-  <si>
-    <t>道具NUM2</t>
+    <t>IconID</t>
+  </si>
+  <si>
+    <t>名字</t>
+  </si>
+  <si>
+    <t>游戏内通用货币</t>
+  </si>
+  <si>
+    <t>属性ID1</t>
+  </si>
+  <si>
+    <t>属性Value1</t>
+  </si>
+  <si>
+    <t>属性ID2</t>
+  </si>
+  <si>
+    <t>属性Value2</t>
+  </si>
+  <si>
+    <t>效果列表</t>
+  </si>
+  <si>
+    <t>活动ID</t>
+  </si>
+  <si>
+    <t>章ID</t>
+  </si>
+  <si>
+    <t>节ID</t>
+  </si>
+  <si>
+    <t>奖励ID1</t>
+  </si>
+  <si>
+    <t>奖励NUM1</t>
+  </si>
+  <si>
+    <t>奖励ID2</t>
+  </si>
+  <si>
+    <t>奖励NUM2</t>
+  </si>
+  <si>
+    <t>签到活动</t>
+  </si>
+  <si>
+    <t>开始时间</t>
+  </si>
+  <si>
+    <t>结束时间</t>
+  </si>
+  <si>
+    <t>2020-10-01  05:00:00</t>
+  </si>
+  <si>
+    <t>抽奖活动</t>
+  </si>
+  <si>
+    <t>月卡活动</t>
+  </si>
+  <si>
+    <t>游戏内支付货币</t>
+  </si>
+  <si>
+    <t>点券</t>
+  </si>
+  <si>
+    <t>宝石</t>
+  </si>
+  <si>
+    <t>游戏内稀有货币</t>
   </si>
 </sst>
 </file>
@@ -436,35 +493,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D8C8FD-A524-2A42-B4E6-70BAC4C065B6}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="10.83203125" style="1"/>
-    <col min="4" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="14.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="2"/>
-    <col min="7" max="7" width="14.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="17" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="10.83203125" style="2"/>
+    <col min="6" max="6" width="14.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="2"/>
+    <col min="8" max="8" width="12.5" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="25.1640625" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>9</v>
@@ -475,40 +535,110 @@
       <c r="G1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>3</v>
+      <c r="H1" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1001</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1">
-        <v>31010</v>
-      </c>
-      <c r="D2" s="2">
-        <v>2001</v>
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5001001</v>
       </c>
       <c r="E2" s="2">
-        <v>1</v>
+        <v>2001</v>
       </c>
       <c r="F2" s="2">
-        <v>2001</v>
+        <v>1</v>
       </c>
       <c r="G2" s="2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>6</v>
+        <v>2001</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1002</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1">
+        <v>5001002</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2001</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2001</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1003</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5001003</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2001</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2001</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -518,70 +648,144 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB9BCC5-DC51-4147-998A-9AFD936B0F72}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="9" max="10" width="25" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>100001</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2001</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2002</v>
+      </c>
+      <c r="H2" s="2">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="J2" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1001</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1">
-        <v>31010</v>
-      </c>
-      <c r="D2" s="2">
-        <v>2001</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2">
-        <v>2001</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>5</v>
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>100002</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2001</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2002</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>100003</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2001</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2002</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: finish conversion of list
</commit_message>
<xml_diff>
--- a/tests/Test.xlsx
+++ b/tests/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wenchyzhu/Github/tableau/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852A33B6-D0D8-F94D-A9D0-00558EF3C2F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0910525-E70E-B042-A76F-87AE7B06C35B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="1620" windowWidth="28040" windowHeight="14740" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="760" yWindow="1620" windowWidth="28040" windowHeight="14740" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -63,18 +63,6 @@
     <t>游戏内通用货币</t>
   </si>
   <si>
-    <t>属性ID1</t>
-  </si>
-  <si>
-    <t>属性Value1</t>
-  </si>
-  <si>
-    <t>属性ID2</t>
-  </si>
-  <si>
-    <t>属性Value2</t>
-  </si>
-  <si>
     <t>效果列表</t>
   </si>
   <si>
@@ -87,18 +75,6 @@
     <t>节ID</t>
   </si>
   <si>
-    <t>奖励ID1</t>
-  </si>
-  <si>
-    <t>奖励NUM1</t>
-  </si>
-  <si>
-    <t>奖励ID2</t>
-  </si>
-  <si>
-    <t>奖励NUM2</t>
-  </si>
-  <si>
     <t>签到活动</t>
   </si>
   <si>
@@ -127,6 +103,30 @@
   </si>
   <si>
     <t>游戏内稀有货币</t>
+  </si>
+  <si>
+    <t>属性1ID</t>
+  </si>
+  <si>
+    <t>属性2Value</t>
+  </si>
+  <si>
+    <t>属性2ID</t>
+  </si>
+  <si>
+    <t>奖励1ID</t>
+  </si>
+  <si>
+    <t>奖励2NUM</t>
+  </si>
+  <si>
+    <t>奖励2ID</t>
+  </si>
+  <si>
+    <t>奖励1NUM</t>
+  </si>
+  <si>
+    <t>属性1Value</t>
   </si>
 </sst>
 </file>
@@ -496,7 +496,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -527,19 +527,19 @@
         <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>2</v>
@@ -582,10 +582,10 @@
         <v>1002</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1">
         <v>5001002</v>
@@ -614,10 +614,10 @@
         <v>1003</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1">
         <v>5001003</v>
@@ -651,7 +651,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -662,34 +662,34 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -703,7 +703,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2">
         <v>2001</v>
@@ -721,7 +721,7 @@
         <v>4</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -735,7 +735,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2">
         <v>2001</v>
@@ -753,7 +753,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -767,7 +767,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E4" s="2">
         <v>2001</v>
@@ -785,7 +785,7 @@
         <v>4</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: process conversion of Timestamp and Duration, test nested message, list, and map
</commit_message>
<xml_diff>
--- a/tests/Test.xlsx
+++ b/tests/Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wenchyzhu/Github/tableau/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061C9AB1-A1D3-0348-B7DB-9ABDBC7671F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AD0E21-9E8E-4C44-909C-56981FCCC442}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="1040" windowWidth="28040" windowHeight="14740" activeTab="1" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="1845" yWindow="5625" windowWidth="31800" windowHeight="12975" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
   <si>
     <t>道具ID</t>
   </si>
@@ -142,6 +140,81 @@
   </si>
   <si>
     <t>月卡活动章1</t>
+  </si>
+  <si>
+    <t>签到活动章2</t>
+  </si>
+  <si>
+    <t>签到活动节2</t>
+  </si>
+  <si>
+    <t>有效多久</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>持续多久</t>
+  </si>
+  <si>
+    <t>属性1强化1ID</t>
+  </si>
+  <si>
+    <t>属性1强化1描述</t>
+  </si>
+  <si>
+    <t>属性1强化1提示列表</t>
+  </si>
+  <si>
+    <t>新,热,限</t>
+  </si>
+  <si>
+    <t>新</t>
+  </si>
+  <si>
+    <t>新,热</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>属性2强化1描述</t>
+  </si>
+  <si>
+    <t>属性2强化1提示列表</t>
+  </si>
+  <si>
+    <t>属性2强化1ID</t>
+  </si>
+  <si>
+    <t>强化2描述1</t>
+  </si>
+  <si>
+    <t>强化2描述2</t>
+  </si>
+  <si>
+    <t>强化2描述3</t>
+  </si>
+  <si>
+    <t>强化1描述1</t>
+  </si>
+  <si>
+    <t>强化1描述2</t>
+  </si>
+  <si>
+    <t>强化1描述3</t>
+  </si>
+  <si>
+    <t>属性1类型</t>
+  </si>
+  <si>
+    <t>属性1数量</t>
+  </si>
+  <si>
+    <t>属性2类型</t>
+  </si>
+  <si>
+    <t>属性2数量</t>
   </si>
 </sst>
 </file>
@@ -196,7 +269,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -212,7 +285,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -508,27 +581,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D8C8FD-A524-2A42-B4E6-70BAC4C065B6}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="1" max="2" width="10.875" style="1"/>
     <col min="3" max="3" width="17" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="10.83203125" style="2"/>
-    <col min="6" max="6" width="14.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="2"/>
-    <col min="8" max="8" width="12.5" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="1"/>
-    <col min="10" max="10" width="25.1640625" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="10.875" style="1"/>
+    <col min="5" max="5" width="10.875" style="2"/>
+    <col min="6" max="8" width="14.375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="19.625" style="2" customWidth="1"/>
+    <col min="10" max="11" width="14.375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="10.875" style="2"/>
+    <col min="13" max="13" width="12.5" style="2" customWidth="1"/>
+    <col min="14" max="15" width="14.375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="19.625" style="2" customWidth="1"/>
+    <col min="17" max="18" width="14.375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="10.875" style="1"/>
+    <col min="20" max="20" width="25.125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="20.875" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,19 +627,52 @@
         <v>27</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="N1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>2</v>
+      <c r="T1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1001</v>
       </c>
@@ -580,19 +692,52 @@
         <v>1</v>
       </c>
       <c r="G2" s="2">
-        <v>2001</v>
-      </c>
-      <c r="H2" s="2">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2">
+        <v>2002</v>
+      </c>
+      <c r="M2" s="2">
+        <v>2</v>
+      </c>
+      <c r="N2" s="2">
+        <v>11</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>1</v>
+      </c>
+      <c r="R2" s="2">
+        <v>5</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1</v>
+      </c>
+      <c r="T2" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="U2" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1002</v>
       </c>
@@ -612,19 +757,52 @@
         <v>1</v>
       </c>
       <c r="G3" s="2">
-        <v>2001</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="2">
+        <v>2</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2">
+        <v>2002</v>
+      </c>
+      <c r="M3" s="2">
+        <v>2</v>
+      </c>
+      <c r="N3" s="2">
+        <v>12</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>2</v>
+      </c>
+      <c r="R3" s="2">
+        <v>6</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="T3" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="U3" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1003</v>
       </c>
@@ -644,16 +822,49 @@
         <v>1</v>
       </c>
       <c r="G4" s="2">
-        <v>2001</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="H4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="2">
+        <v>3</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
+        <v>2002</v>
+      </c>
+      <c r="M4" s="2">
+        <v>2</v>
+      </c>
+      <c r="N4" s="2">
+        <v>13</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>3</v>
+      </c>
+      <c r="R4" s="2">
+        <v>7</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="T4" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -663,20 +874,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB9BCC5-DC51-4147-998A-9AFD936B0F72}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.83203125" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.875" customWidth="1"/>
+    <col min="5" max="5" width="23.875" customWidth="1"/>
     <col min="10" max="11" width="25" customWidth="1"/>
+    <col min="12" max="12" width="20.875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -710,8 +922,11 @@
       <c r="K1" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>100001</v>
       </c>
@@ -745,22 +960,25 @@
       <c r="K2" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="L2" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>100002</v>
+        <v>100001</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F3" s="2">
         <v>2001</v>
@@ -780,40 +998,122 @@
       <c r="K3" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="L3" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>100003</v>
+        <v>100001</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F4" s="2">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="G4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4" s="2">
         <v>2002</v>
       </c>
       <c r="I4" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>15</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>100002</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2001</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2002</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>100003</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2001</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2002</v>
+      </c>
+      <c r="I6" s="2">
+        <v>2</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: support simple in-cell Map
</commit_message>
<xml_diff>
--- a/tests/Test.xlsx
+++ b/tests/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AD0E21-9E8E-4C44-909C-56981FCCC442}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC047D0A-EBA0-4640-AC4A-1DC7B3BA8D09}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1845" yWindow="5625" windowWidth="31800" windowHeight="12975" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="-2730" yWindow="3405" windowWidth="37020" windowHeight="13740" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="65">
   <si>
     <t>道具ID</t>
   </si>
@@ -215,6 +215,18 @@
   </si>
   <si>
     <t>属性2数量</t>
+  </si>
+  <si>
+    <t>售卖选项</t>
+  </si>
+  <si>
+    <t>1:15,2:500</t>
+  </si>
+  <si>
+    <t>1:10</t>
+  </si>
+  <si>
+    <t>1:50,2:900,3:2000</t>
   </si>
 </sst>
 </file>
@@ -581,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D8C8FD-A524-2A42-B4E6-70BAC4C065B6}">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -602,12 +614,13 @@
     <col min="16" max="16" width="19.625" style="2" customWidth="1"/>
     <col min="17" max="18" width="14.375" style="2" customWidth="1"/>
     <col min="19" max="19" width="10.875" style="1"/>
-    <col min="20" max="20" width="25.125" style="3" customWidth="1"/>
-    <col min="21" max="21" width="20.875" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="10.875" style="1"/>
+    <col min="20" max="20" width="24.5" style="3" customWidth="1"/>
+    <col min="21" max="21" width="25.125" style="3" customWidth="1"/>
+    <col min="22" max="22" width="20.875" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -666,13 +679,16 @@
         <v>9</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1001</v>
       </c>
@@ -731,13 +747,16 @@
         <v>1</v>
       </c>
       <c r="T2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1002</v>
       </c>
@@ -796,13 +815,16 @@
         <v>47</v>
       </c>
       <c r="T3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="U3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1003</v>
       </c>
@@ -861,14 +883,18 @@
         <v>3</v>
       </c>
       <c r="T4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="U4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>